<commit_message>
Dapper implemmented for getting student dashboard list
</commit_message>
<xml_diff>
--- a/staff-student-API/Root/Excel/Mark2.xlsx
+++ b/staff-student-API/Root/Excel/Mark2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dotnetcore samples\Staff and student management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34C4B02-7426-4431-9BF9-D00CEBB9791B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03376051-6E7A-448C-854A-F8408D3A98EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="660" windowWidth="15375" windowHeight="7875" xr2:uid="{50FB4ECA-94E0-44B4-9514-F8F6417F74A6}"/>
   </bookViews>
@@ -443,7 +443,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12001</v>
+        <v>1001</v>
       </c>
       <c r="B2">
         <v>96</v>

</xml_diff>